<commit_message>
refactor: enhance ESLint configuration and add individual/group inscription features
- Updated ESLint configuration to include Prettier and unused imports plugins for improved code quality.
- Added custom scrollbar styles to global CSS for better UI consistency.
- Implemented new components and hooks for individual and group inscription processes, including forms and confirmation pages.
- Enhanced user experience with loading states, error handling, and improved navigation in the user interface.
- Introduced API functions for managing individual and group inscriptions, ensuring robust data handling.
</commit_message>
<xml_diff>
--- a/public/xlsx/Inscrições Aperfeiçoamento para Serviços.xlsx
+++ b/public/xlsx/Inscrições Aperfeiçoamento para Serviços.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>LISTA DE INSCRIÇÕES</t>
   </si>
@@ -64,6 +64,9 @@
 (formato DD/MM/AAAA)</t>
   </si>
   <si>
+    <t>Sexo</t>
+  </si>
+  <si>
     <t>Tipo Inscrição</t>
   </si>
   <si>
@@ -83,10 +86,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$R$ -416]#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="dd/MM/yyyy"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -117,6 +121,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="10.0"/>
       <color theme="1"/>
@@ -131,6 +140,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10.0"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -162,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -175,24 +185,30 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -416,7 +432,8 @@
     <col customWidth="1" min="1" max="1" width="16.5"/>
     <col customWidth="1" min="2" max="2" width="25.0"/>
     <col customWidth="1" min="3" max="3" width="29.75"/>
-    <col customWidth="1" min="4" max="4" width="28.38"/>
+    <col customWidth="1" min="4" max="4" width="22.0"/>
+    <col customWidth="1" min="5" max="5" width="17.75"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -430,1049 +447,1359 @@
       </c>
     </row>
     <row r="3">
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="3"/>
+      <c r="E3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="4">
-        <f>SUM(E6:E1000)</f>
+      <c r="F3" s="5">
+        <f>SUM(F6:F1000)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="8" t="s">
         <v>8</v>
       </c>
+      <c r="F5" s="8" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="8">
+      <c r="A6" s="9">
         <v>1.0</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="10">
-        <f>IFERROR(VLOOKUP(D6, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="11">
+        <f>IFERROR(VLOOKUP(E6, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="8">
+      <c r="A7" s="9">
         <v>2.0</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="10">
-        <f>IFERROR(VLOOKUP(D7, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="11">
+        <f>IFERROR(VLOOKUP(E7, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="8">
+      <c r="A8" s="9">
         <v>3.0</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="10">
-        <f>IFERROR(VLOOKUP(D8, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B8" s="12"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="11">
+        <f>IFERROR(VLOOKUP(E8, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="8">
+      <c r="A9" s="9">
         <v>4.0</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="10">
-        <f>IFERROR(VLOOKUP(D9, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B9" s="12"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="11">
+        <f>IFERROR(VLOOKUP(E9, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="8">
+      <c r="A10" s="9">
         <v>5.0</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="10">
-        <f>IFERROR(VLOOKUP(D10, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B10" s="12"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="11">
+        <f>IFERROR(VLOOKUP(E10, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="8">
+      <c r="A11" s="9">
         <v>6.0</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="10">
-        <f>IFERROR(VLOOKUP(D11, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B11" s="12"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="11">
+        <f>IFERROR(VLOOKUP(E11, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="8">
+      <c r="A12" s="9">
         <v>7.0</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="10">
-        <f>IFERROR(VLOOKUP(D12, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B12" s="12"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="11">
+        <f>IFERROR(VLOOKUP(E12, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="8">
+      <c r="A13" s="9">
         <v>8.0</v>
       </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="10">
-        <f>IFERROR(VLOOKUP(D13, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B13" s="12"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="11">
+        <f>IFERROR(VLOOKUP(E13, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="8">
+      <c r="A14" s="9">
         <v>9.0</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="10">
-        <f>IFERROR(VLOOKUP(D14, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B14" s="12"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="11">
+        <f>IFERROR(VLOOKUP(E14, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="8">
+      <c r="A15" s="9">
         <v>10.0</v>
       </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="10">
-        <f>IFERROR(VLOOKUP(D15, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B15" s="12"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="11">
+        <f>IFERROR(VLOOKUP(E15, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="8">
+      <c r="A16" s="9">
         <v>11.0</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="10">
-        <f>IFERROR(VLOOKUP(D16, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B16" s="12"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="11">
+        <f>IFERROR(VLOOKUP(E16, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="8">
+      <c r="A17" s="9">
         <v>12.0</v>
       </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="10">
-        <f>IFERROR(VLOOKUP(D17, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B17" s="12"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="11">
+        <f>IFERROR(VLOOKUP(E17, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="8">
+      <c r="A18" s="9">
         <v>13.0</v>
       </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="10">
-        <f>IFERROR(VLOOKUP(D18, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B18" s="12"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="11">
+        <f>IFERROR(VLOOKUP(E18, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="8">
+      <c r="A19" s="9">
         <v>14.0</v>
       </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="10">
-        <f>IFERROR(VLOOKUP(D19, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B19" s="12"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="11">
+        <f>IFERROR(VLOOKUP(E19, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="8">
+      <c r="A20" s="9">
         <v>15.0</v>
       </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="10">
-        <f>IFERROR(VLOOKUP(D20, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B20" s="12"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="11">
+        <f>IFERROR(VLOOKUP(E20, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="8">
+      <c r="A21" s="9">
         <v>16.0</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="10">
-        <f>IFERROR(VLOOKUP(D21, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B21" s="12"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="11">
+        <f>IFERROR(VLOOKUP(E21, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="8">
+      <c r="A22" s="9">
         <v>17.0</v>
       </c>
-      <c r="D22" s="11"/>
-      <c r="E22" s="10">
-        <f>IFERROR(VLOOKUP(D22, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B22" s="12"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="11">
+        <f>IFERROR(VLOOKUP(E22, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="8">
+      <c r="A23" s="9">
         <v>18.0</v>
       </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="10">
-        <f>IFERROR(VLOOKUP(D23, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B23" s="12"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="11">
+        <f>IFERROR(VLOOKUP(E23, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="8">
+      <c r="A24" s="9">
         <v>19.0</v>
       </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="10">
-        <f>IFERROR(VLOOKUP(D24, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B24" s="12"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="11">
+        <f>IFERROR(VLOOKUP(E24, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="8">
+      <c r="A25" s="9">
         <v>20.0</v>
       </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="10">
-        <f>IFERROR(VLOOKUP(D25, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B25" s="12"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="11">
+        <f>IFERROR(VLOOKUP(E25, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="8">
+      <c r="A26" s="9">
         <v>21.0</v>
       </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="10">
-        <f>IFERROR(VLOOKUP(D26, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B26" s="12"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="11">
+        <f>IFERROR(VLOOKUP(E26, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="8">
+      <c r="A27" s="9">
         <v>22.0</v>
       </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="10">
-        <f>IFERROR(VLOOKUP(D27, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B27" s="12"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="11">
+        <f>IFERROR(VLOOKUP(E27, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="8">
+      <c r="A28" s="9">
         <v>23.0</v>
       </c>
-      <c r="D28" s="11"/>
-      <c r="E28" s="10">
-        <f>IFERROR(VLOOKUP(D28, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B28" s="12"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="11">
+        <f>IFERROR(VLOOKUP(E28, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="8">
+      <c r="A29" s="9">
         <v>24.0</v>
       </c>
-      <c r="D29" s="11"/>
-      <c r="E29" s="10">
-        <f>IFERROR(VLOOKUP(D29, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B29" s="12"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="11">
+        <f>IFERROR(VLOOKUP(E29, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="8">
+      <c r="A30" s="9">
         <v>25.0</v>
       </c>
-      <c r="D30" s="11"/>
-      <c r="E30" s="10">
-        <f>IFERROR(VLOOKUP(D30, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B30" s="12"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="11">
+        <f>IFERROR(VLOOKUP(E30, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="8">
+      <c r="A31" s="9">
         <v>26.0</v>
       </c>
-      <c r="D31" s="11"/>
-      <c r="E31" s="10">
-        <f>IFERROR(VLOOKUP(D31, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B31" s="12"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="11">
+        <f>IFERROR(VLOOKUP(E31, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="8">
+      <c r="A32" s="9">
         <v>27.0</v>
       </c>
-      <c r="D32" s="11"/>
-      <c r="E32" s="10">
-        <f>IFERROR(VLOOKUP(D32, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B32" s="12"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="11">
+        <f>IFERROR(VLOOKUP(E32, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="8">
+      <c r="A33" s="9">
         <v>28.0</v>
       </c>
-      <c r="D33" s="11"/>
-      <c r="E33" s="10">
-        <f>IFERROR(VLOOKUP(D33, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B33" s="12"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="11">
+        <f>IFERROR(VLOOKUP(E33, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="8">
+      <c r="A34" s="9">
         <v>29.0</v>
       </c>
-      <c r="D34" s="11"/>
-      <c r="E34" s="10">
-        <f>IFERROR(VLOOKUP(D34, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B34" s="12"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="11">
+        <f>IFERROR(VLOOKUP(E34, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="8">
+      <c r="A35" s="9">
         <v>30.0</v>
       </c>
-      <c r="D35" s="11"/>
-      <c r="E35" s="10">
-        <f>IFERROR(VLOOKUP(D35, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B35" s="12"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="11">
+        <f>IFERROR(VLOOKUP(E35, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="8">
+      <c r="A36" s="9">
         <v>31.0</v>
       </c>
-      <c r="D36" s="11"/>
-      <c r="E36" s="10">
-        <f>IFERROR(VLOOKUP(D36, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B36" s="12"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="11">
+        <f>IFERROR(VLOOKUP(E36, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="8">
+      <c r="A37" s="9">
         <v>32.0</v>
       </c>
-      <c r="D37" s="11"/>
-      <c r="E37" s="10">
-        <f>IFERROR(VLOOKUP(D37, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B37" s="12"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="11">
+        <f>IFERROR(VLOOKUP(E37, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="8">
+      <c r="A38" s="9">
         <v>33.0</v>
       </c>
-      <c r="D38" s="11"/>
-      <c r="E38" s="10">
-        <f>IFERROR(VLOOKUP(D38, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B38" s="12"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="11">
+        <f>IFERROR(VLOOKUP(E38, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="8">
+      <c r="A39" s="9">
         <v>34.0</v>
       </c>
-      <c r="D39" s="11"/>
-      <c r="E39" s="10">
-        <f>IFERROR(VLOOKUP(D39, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B39" s="12"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="11">
+        <f>IFERROR(VLOOKUP(E39, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="8">
+      <c r="A40" s="9">
         <v>35.0</v>
       </c>
-      <c r="D40" s="11"/>
-      <c r="E40" s="10">
-        <f>IFERROR(VLOOKUP(D40, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B40" s="12"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="11">
+        <f>IFERROR(VLOOKUP(E40, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="8">
+      <c r="A41" s="9">
         <v>36.0</v>
       </c>
-      <c r="D41" s="11"/>
-      <c r="E41" s="10">
-        <f>IFERROR(VLOOKUP(D41, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B41" s="12"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="11">
+        <f>IFERROR(VLOOKUP(E41, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="8">
+      <c r="A42" s="9">
         <v>37.0</v>
       </c>
-      <c r="D42" s="11"/>
-      <c r="E42" s="10">
-        <f>IFERROR(VLOOKUP(D42, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B42" s="12"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="11">
+        <f>IFERROR(VLOOKUP(E42, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="8">
+      <c r="A43" s="9">
         <v>38.0</v>
       </c>
-      <c r="D43" s="11"/>
-      <c r="E43" s="10">
-        <f>IFERROR(VLOOKUP(D43, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B43" s="12"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="11">
+        <f>IFERROR(VLOOKUP(E43, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="8">
+      <c r="A44" s="9">
         <v>39.0</v>
       </c>
-      <c r="D44" s="11"/>
-      <c r="E44" s="10">
-        <f>IFERROR(VLOOKUP(D44, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B44" s="12"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="11">
+        <f>IFERROR(VLOOKUP(E44, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="8">
+      <c r="A45" s="9">
         <v>40.0</v>
       </c>
-      <c r="D45" s="11"/>
-      <c r="E45" s="10">
-        <f>IFERROR(VLOOKUP(D45, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B45" s="12"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="11">
+        <f>IFERROR(VLOOKUP(E45, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="8">
+      <c r="A46" s="9">
         <v>41.0</v>
       </c>
-      <c r="D46" s="11"/>
-      <c r="E46" s="10">
-        <f>IFERROR(VLOOKUP(D46, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B46" s="12"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="11">
+        <f>IFERROR(VLOOKUP(E46, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="8">
+      <c r="A47" s="9">
         <v>42.0</v>
       </c>
-      <c r="D47" s="11"/>
-      <c r="E47" s="10">
-        <f>IFERROR(VLOOKUP(D47, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B47" s="12"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="11">
+        <f>IFERROR(VLOOKUP(E47, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="8">
+      <c r="A48" s="9">
         <v>43.0</v>
       </c>
-      <c r="D48" s="11"/>
-      <c r="E48" s="10">
-        <f>IFERROR(VLOOKUP(D48, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B48" s="12"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="11">
+        <f>IFERROR(VLOOKUP(E48, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="8">
+      <c r="A49" s="9">
         <v>44.0</v>
       </c>
-      <c r="D49" s="11"/>
-      <c r="E49" s="10">
-        <f>IFERROR(VLOOKUP(D49, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B49" s="12"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="11">
+        <f>IFERROR(VLOOKUP(E49, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="8">
+      <c r="A50" s="9">
         <v>45.0</v>
       </c>
-      <c r="D50" s="11"/>
-      <c r="E50" s="10">
-        <f>IFERROR(VLOOKUP(D50, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B50" s="12"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="11">
+        <f>IFERROR(VLOOKUP(E50, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="8">
+      <c r="A51" s="9">
         <v>46.0</v>
       </c>
-      <c r="D51" s="11"/>
-      <c r="E51" s="10">
-        <f>IFERROR(VLOOKUP(D51, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B51" s="12"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="11">
+        <f>IFERROR(VLOOKUP(E51, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="8">
+      <c r="A52" s="9">
         <v>47.0</v>
       </c>
-      <c r="D52" s="11"/>
-      <c r="E52" s="10">
-        <f>IFERROR(VLOOKUP(D52, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B52" s="12"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="11">
+        <f>IFERROR(VLOOKUP(E52, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="8">
+      <c r="A53" s="9">
         <v>48.0</v>
       </c>
-      <c r="D53" s="11"/>
-      <c r="E53" s="10">
-        <f>IFERROR(VLOOKUP(D53, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B53" s="12"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="11">
+        <f>IFERROR(VLOOKUP(E53, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="8">
+      <c r="A54" s="9">
         <v>49.0</v>
       </c>
-      <c r="D54" s="11"/>
-      <c r="E54" s="10">
-        <f>IFERROR(VLOOKUP(D54, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B54" s="12"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="11">
+        <f>IFERROR(VLOOKUP(E54, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="8">
+      <c r="A55" s="9">
         <v>50.0</v>
       </c>
-      <c r="D55" s="11"/>
-      <c r="E55" s="10">
-        <f>IFERROR(VLOOKUP(D55, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B55" s="12"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="11">
+        <f>IFERROR(VLOOKUP(E55, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="8">
+      <c r="A56" s="9">
         <v>51.0</v>
       </c>
-      <c r="D56" s="11"/>
-      <c r="E56" s="10">
-        <f>IFERROR(VLOOKUP(D56, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B56" s="12"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="11">
+        <f>IFERROR(VLOOKUP(E56, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="8">
+      <c r="A57" s="9">
         <v>52.0</v>
       </c>
-      <c r="D57" s="11"/>
-      <c r="E57" s="10">
-        <f>IFERROR(VLOOKUP(D57, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B57" s="12"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="12"/>
+      <c r="F57" s="11">
+        <f>IFERROR(VLOOKUP(E57, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="8">
+      <c r="A58" s="9">
         <v>53.0</v>
       </c>
-      <c r="D58" s="11"/>
-      <c r="E58" s="10">
-        <f>IFERROR(VLOOKUP(D58, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B58" s="12"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="11">
+        <f>IFERROR(VLOOKUP(E58, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="8">
+      <c r="A59" s="9">
         <v>54.0</v>
       </c>
-      <c r="D59" s="11"/>
-      <c r="E59" s="10">
-        <f>IFERROR(VLOOKUP(D59, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B59" s="12"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12"/>
+      <c r="F59" s="11">
+        <f>IFERROR(VLOOKUP(E59, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="8">
+      <c r="A60" s="9">
         <v>55.0</v>
       </c>
-      <c r="D60" s="11"/>
-      <c r="E60" s="10">
-        <f>IFERROR(VLOOKUP(D60, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B60" s="12"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="11">
+        <f>IFERROR(VLOOKUP(E60, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="8">
+      <c r="A61" s="9">
         <v>56.0</v>
       </c>
-      <c r="D61" s="11"/>
-      <c r="E61" s="10">
-        <f>IFERROR(VLOOKUP(D61, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B61" s="12"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="11">
+        <f>IFERROR(VLOOKUP(E61, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="8">
+      <c r="A62" s="9">
         <v>57.0</v>
       </c>
-      <c r="D62" s="11"/>
-      <c r="E62" s="10">
-        <f>IFERROR(VLOOKUP(D62, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B62" s="12"/>
+      <c r="C62" s="10"/>
+      <c r="D62" s="12"/>
+      <c r="E62" s="12"/>
+      <c r="F62" s="11">
+        <f>IFERROR(VLOOKUP(E62, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="8">
+      <c r="A63" s="9">
         <v>58.0</v>
       </c>
-      <c r="D63" s="11"/>
-      <c r="E63" s="10">
-        <f>IFERROR(VLOOKUP(D63, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B63" s="12"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="12"/>
+      <c r="E63" s="12"/>
+      <c r="F63" s="11">
+        <f>IFERROR(VLOOKUP(E63, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="8">
+      <c r="A64" s="9">
         <v>59.0</v>
       </c>
-      <c r="D64" s="11"/>
-      <c r="E64" s="10">
-        <f>IFERROR(VLOOKUP(D64, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B64" s="12"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="12"/>
+      <c r="F64" s="11">
+        <f>IFERROR(VLOOKUP(E64, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="8">
+      <c r="A65" s="9">
         <v>60.0</v>
       </c>
-      <c r="D65" s="11"/>
-      <c r="E65" s="10">
-        <f>IFERROR(VLOOKUP(D65, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B65" s="12"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="11">
+        <f>IFERROR(VLOOKUP(E65, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="8">
+      <c r="A66" s="9">
         <v>61.0</v>
       </c>
-      <c r="D66" s="11"/>
-      <c r="E66" s="10">
-        <f>IFERROR(VLOOKUP(D66, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B66" s="12"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="12"/>
+      <c r="E66" s="12"/>
+      <c r="F66" s="11">
+        <f>IFERROR(VLOOKUP(E66, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="8">
+      <c r="A67" s="9">
         <v>62.0</v>
       </c>
-      <c r="D67" s="11"/>
-      <c r="E67" s="10">
-        <f>IFERROR(VLOOKUP(D67, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B67" s="12"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="12"/>
+      <c r="F67" s="11">
+        <f>IFERROR(VLOOKUP(E67, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="8">
+      <c r="A68" s="9">
         <v>63.0</v>
       </c>
-      <c r="D68" s="11"/>
-      <c r="E68" s="10">
-        <f>IFERROR(VLOOKUP(D68, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B68" s="12"/>
+      <c r="C68" s="10"/>
+      <c r="D68" s="12"/>
+      <c r="E68" s="12"/>
+      <c r="F68" s="11">
+        <f>IFERROR(VLOOKUP(E68, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="8">
+      <c r="A69" s="9">
         <v>64.0</v>
       </c>
-      <c r="D69" s="11"/>
-      <c r="E69" s="10">
-        <f>IFERROR(VLOOKUP(D69, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B69" s="12"/>
+      <c r="C69" s="10"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="12"/>
+      <c r="F69" s="11">
+        <f>IFERROR(VLOOKUP(E69, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="8">
+      <c r="A70" s="9">
         <v>65.0</v>
       </c>
-      <c r="D70" s="11"/>
-      <c r="E70" s="10">
-        <f>IFERROR(VLOOKUP(D70, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B70" s="12"/>
+      <c r="C70" s="10"/>
+      <c r="D70" s="12"/>
+      <c r="E70" s="12"/>
+      <c r="F70" s="11">
+        <f>IFERROR(VLOOKUP(E70, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="8">
+      <c r="A71" s="9">
         <v>66.0</v>
       </c>
-      <c r="D71" s="11"/>
-      <c r="E71" s="10">
-        <f>IFERROR(VLOOKUP(D71, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B71" s="12"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="12"/>
+      <c r="E71" s="12"/>
+      <c r="F71" s="11">
+        <f>IFERROR(VLOOKUP(E71, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="8">
+      <c r="A72" s="9">
         <v>67.0</v>
       </c>
-      <c r="D72" s="11"/>
-      <c r="E72" s="10">
-        <f>IFERROR(VLOOKUP(D72, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B72" s="12"/>
+      <c r="C72" s="10"/>
+      <c r="D72" s="12"/>
+      <c r="E72" s="12"/>
+      <c r="F72" s="11">
+        <f>IFERROR(VLOOKUP(E72, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="8">
+      <c r="A73" s="9">
         <v>68.0</v>
       </c>
-      <c r="D73" s="11"/>
-      <c r="E73" s="10">
-        <f>IFERROR(VLOOKUP(D73, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B73" s="12"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="12"/>
+      <c r="E73" s="12"/>
+      <c r="F73" s="11">
+        <f>IFERROR(VLOOKUP(E73, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="8">
+      <c r="A74" s="9">
         <v>69.0</v>
       </c>
-      <c r="D74" s="11"/>
-      <c r="E74" s="10">
-        <f>IFERROR(VLOOKUP(D74, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B74" s="12"/>
+      <c r="C74" s="10"/>
+      <c r="D74" s="12"/>
+      <c r="E74" s="12"/>
+      <c r="F74" s="11">
+        <f>IFERROR(VLOOKUP(E74, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="8">
+      <c r="A75" s="9">
         <v>70.0</v>
       </c>
-      <c r="D75" s="11"/>
-      <c r="E75" s="10">
-        <f>IFERROR(VLOOKUP(D75, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B75" s="12"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="12"/>
+      <c r="E75" s="12"/>
+      <c r="F75" s="11">
+        <f>IFERROR(VLOOKUP(E75, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="8">
+      <c r="A76" s="9">
         <v>71.0</v>
       </c>
-      <c r="D76" s="11"/>
-      <c r="E76" s="10">
-        <f>IFERROR(VLOOKUP(D76, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B76" s="12"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="12"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="11">
+        <f>IFERROR(VLOOKUP(E76, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="8">
+      <c r="A77" s="9">
         <v>72.0</v>
       </c>
-      <c r="D77" s="11"/>
-      <c r="E77" s="10">
-        <f>IFERROR(VLOOKUP(D77, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B77" s="12"/>
+      <c r="C77" s="10"/>
+      <c r="D77" s="12"/>
+      <c r="E77" s="12"/>
+      <c r="F77" s="11">
+        <f>IFERROR(VLOOKUP(E77, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="8">
+      <c r="A78" s="9">
         <v>73.0</v>
       </c>
-      <c r="D78" s="11"/>
-      <c r="E78" s="10">
-        <f>IFERROR(VLOOKUP(D78, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B78" s="12"/>
+      <c r="C78" s="10"/>
+      <c r="D78" s="12"/>
+      <c r="E78" s="12"/>
+      <c r="F78" s="11">
+        <f>IFERROR(VLOOKUP(E78, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="8">
+      <c r="A79" s="9">
         <v>74.0</v>
       </c>
-      <c r="D79" s="11"/>
-      <c r="E79" s="10">
-        <f>IFERROR(VLOOKUP(D79, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B79" s="12"/>
+      <c r="C79" s="10"/>
+      <c r="D79" s="12"/>
+      <c r="E79" s="12"/>
+      <c r="F79" s="11">
+        <f>IFERROR(VLOOKUP(E79, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="8">
+      <c r="A80" s="9">
         <v>75.0</v>
       </c>
-      <c r="D80" s="11"/>
-      <c r="E80" s="10">
-        <f>IFERROR(VLOOKUP(D80, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B80" s="12"/>
+      <c r="C80" s="10"/>
+      <c r="D80" s="12"/>
+      <c r="E80" s="12"/>
+      <c r="F80" s="11">
+        <f>IFERROR(VLOOKUP(E80, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="8">
+      <c r="A81" s="9">
         <v>76.0</v>
       </c>
-      <c r="D81" s="11"/>
-      <c r="E81" s="10">
-        <f>IFERROR(VLOOKUP(D81, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B81" s="12"/>
+      <c r="C81" s="10"/>
+      <c r="D81" s="12"/>
+      <c r="E81" s="12"/>
+      <c r="F81" s="11">
+        <f>IFERROR(VLOOKUP(E81, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="8">
+      <c r="A82" s="9">
         <v>77.0</v>
       </c>
-      <c r="D82" s="11"/>
-      <c r="E82" s="10">
-        <f>IFERROR(VLOOKUP(D82, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B82" s="12"/>
+      <c r="C82" s="10"/>
+      <c r="D82" s="12"/>
+      <c r="E82" s="12"/>
+      <c r="F82" s="11">
+        <f>IFERROR(VLOOKUP(E82, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="8">
+      <c r="A83" s="9">
         <v>78.0</v>
       </c>
-      <c r="D83" s="11"/>
-      <c r="E83" s="10">
-        <f>IFERROR(VLOOKUP(D83, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B83" s="12"/>
+      <c r="C83" s="10"/>
+      <c r="D83" s="12"/>
+      <c r="E83" s="12"/>
+      <c r="F83" s="11">
+        <f>IFERROR(VLOOKUP(E83, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="8">
+      <c r="A84" s="9">
         <v>79.0</v>
       </c>
-      <c r="D84" s="11"/>
-      <c r="E84" s="10">
-        <f>IFERROR(VLOOKUP(D84, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B84" s="12"/>
+      <c r="C84" s="10"/>
+      <c r="D84" s="12"/>
+      <c r="E84" s="12"/>
+      <c r="F84" s="11">
+        <f>IFERROR(VLOOKUP(E84, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="8">
+      <c r="A85" s="9">
         <v>80.0</v>
       </c>
-      <c r="D85" s="11"/>
-      <c r="E85" s="10">
-        <f>IFERROR(VLOOKUP(D85, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B85" s="12"/>
+      <c r="C85" s="10"/>
+      <c r="D85" s="12"/>
+      <c r="E85" s="12"/>
+      <c r="F85" s="11">
+        <f>IFERROR(VLOOKUP(E85, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="8">
+      <c r="A86" s="9">
         <v>81.0</v>
       </c>
-      <c r="D86" s="11"/>
-      <c r="E86" s="10">
-        <f>IFERROR(VLOOKUP(D86, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B86" s="12"/>
+      <c r="C86" s="10"/>
+      <c r="D86" s="12"/>
+      <c r="E86" s="12"/>
+      <c r="F86" s="11">
+        <f>IFERROR(VLOOKUP(E86, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="8">
+      <c r="A87" s="9">
         <v>82.0</v>
       </c>
-      <c r="D87" s="11"/>
-      <c r="E87" s="10">
-        <f>IFERROR(VLOOKUP(D87, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B87" s="12"/>
+      <c r="C87" s="10"/>
+      <c r="D87" s="12"/>
+      <c r="E87" s="12"/>
+      <c r="F87" s="11">
+        <f>IFERROR(VLOOKUP(E87, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="8">
+      <c r="A88" s="9">
         <v>83.0</v>
       </c>
-      <c r="D88" s="11"/>
-      <c r="E88" s="10">
-        <f>IFERROR(VLOOKUP(D88, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B88" s="12"/>
+      <c r="C88" s="10"/>
+      <c r="D88" s="12"/>
+      <c r="E88" s="12"/>
+      <c r="F88" s="11">
+        <f>IFERROR(VLOOKUP(E88, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="8">
+      <c r="A89" s="9">
         <v>84.0</v>
       </c>
-      <c r="D89" s="11"/>
-      <c r="E89" s="10">
-        <f>IFERROR(VLOOKUP(D89, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B89" s="12"/>
+      <c r="C89" s="10"/>
+      <c r="D89" s="12"/>
+      <c r="E89" s="12"/>
+      <c r="F89" s="11">
+        <f>IFERROR(VLOOKUP(E89, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="8">
+      <c r="A90" s="9">
         <v>85.0</v>
       </c>
-      <c r="D90" s="11"/>
-      <c r="E90" s="10">
-        <f>IFERROR(VLOOKUP(D90, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B90" s="12"/>
+      <c r="C90" s="10"/>
+      <c r="D90" s="12"/>
+      <c r="E90" s="12"/>
+      <c r="F90" s="11">
+        <f>IFERROR(VLOOKUP(E90, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="8">
+      <c r="A91" s="9">
         <v>86.0</v>
       </c>
-      <c r="D91" s="11"/>
-      <c r="E91" s="10">
-        <f>IFERROR(VLOOKUP(D91, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B91" s="12"/>
+      <c r="C91" s="10"/>
+      <c r="D91" s="12"/>
+      <c r="E91" s="12"/>
+      <c r="F91" s="11">
+        <f>IFERROR(VLOOKUP(E91, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="8">
+      <c r="A92" s="9">
         <v>87.0</v>
       </c>
-      <c r="D92" s="11"/>
-      <c r="E92" s="10">
-        <f>IFERROR(VLOOKUP(D92, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B92" s="12"/>
+      <c r="C92" s="10"/>
+      <c r="D92" s="12"/>
+      <c r="E92" s="12"/>
+      <c r="F92" s="11">
+        <f>IFERROR(VLOOKUP(E92, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="8">
+      <c r="A93" s="9">
         <v>88.0</v>
       </c>
-      <c r="D93" s="11"/>
-      <c r="E93" s="10">
-        <f>IFERROR(VLOOKUP(D93, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B93" s="12"/>
+      <c r="C93" s="10"/>
+      <c r="D93" s="12"/>
+      <c r="E93" s="12"/>
+      <c r="F93" s="11">
+        <f>IFERROR(VLOOKUP(E93, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="8">
+      <c r="A94" s="9">
         <v>89.0</v>
       </c>
-      <c r="D94" s="11"/>
-      <c r="E94" s="10">
-        <f>IFERROR(VLOOKUP(D94, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B94" s="12"/>
+      <c r="C94" s="10"/>
+      <c r="D94" s="12"/>
+      <c r="E94" s="12"/>
+      <c r="F94" s="11">
+        <f>IFERROR(VLOOKUP(E94, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="8">
+      <c r="A95" s="9">
         <v>90.0</v>
       </c>
-      <c r="D95" s="11"/>
-      <c r="E95" s="10">
-        <f>IFERROR(VLOOKUP(D95, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B95" s="12"/>
+      <c r="C95" s="10"/>
+      <c r="D95" s="12"/>
+      <c r="E95" s="12"/>
+      <c r="F95" s="11">
+        <f>IFERROR(VLOOKUP(E95, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="8">
+      <c r="A96" s="9">
         <v>91.0</v>
       </c>
-      <c r="D96" s="11"/>
-      <c r="E96" s="10">
-        <f>IFERROR(VLOOKUP(D96, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B96" s="12"/>
+      <c r="C96" s="10"/>
+      <c r="D96" s="12"/>
+      <c r="E96" s="12"/>
+      <c r="F96" s="11">
+        <f>IFERROR(VLOOKUP(E96, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="8">
+      <c r="A97" s="9">
         <v>92.0</v>
       </c>
-      <c r="D97" s="11"/>
-      <c r="E97" s="10">
-        <f>IFERROR(VLOOKUP(D97, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B97" s="12"/>
+      <c r="C97" s="10"/>
+      <c r="D97" s="12"/>
+      <c r="E97" s="12"/>
+      <c r="F97" s="11">
+        <f>IFERROR(VLOOKUP(E97, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="8">
+      <c r="A98" s="9">
         <v>93.0</v>
       </c>
-      <c r="D98" s="11"/>
-      <c r="E98" s="10">
-        <f>IFERROR(VLOOKUP(D98, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B98" s="12"/>
+      <c r="C98" s="10"/>
+      <c r="D98" s="12"/>
+      <c r="E98" s="12"/>
+      <c r="F98" s="11">
+        <f>IFERROR(VLOOKUP(E98, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="8">
+      <c r="A99" s="9">
         <v>94.0</v>
       </c>
-      <c r="D99" s="11"/>
-      <c r="E99" s="10">
-        <f>IFERROR(VLOOKUP(D99, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B99" s="12"/>
+      <c r="C99" s="10"/>
+      <c r="D99" s="12"/>
+      <c r="E99" s="12"/>
+      <c r="F99" s="11">
+        <f>IFERROR(VLOOKUP(E99, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="8">
+      <c r="A100" s="9">
         <v>95.0</v>
       </c>
-      <c r="D100" s="11"/>
-      <c r="E100" s="10">
-        <f>IFERROR(VLOOKUP(D100, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B100" s="12"/>
+      <c r="C100" s="10"/>
+      <c r="D100" s="12"/>
+      <c r="E100" s="12"/>
+      <c r="F100" s="11">
+        <f>IFERROR(VLOOKUP(E100, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="8">
+      <c r="A101" s="9">
         <v>96.0</v>
       </c>
-      <c r="D101" s="11"/>
-      <c r="E101" s="10">
-        <f>IFERROR(VLOOKUP(D101, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B101" s="12"/>
+      <c r="C101" s="10"/>
+      <c r="D101" s="12"/>
+      <c r="E101" s="12"/>
+      <c r="F101" s="11">
+        <f>IFERROR(VLOOKUP(E101, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="8">
+      <c r="A102" s="9">
         <v>97.0</v>
       </c>
-      <c r="D102" s="11"/>
-      <c r="E102" s="10">
-        <f>IFERROR(VLOOKUP(D102, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B102" s="12"/>
+      <c r="C102" s="10"/>
+      <c r="D102" s="12"/>
+      <c r="E102" s="12"/>
+      <c r="F102" s="11">
+        <f>IFERROR(VLOOKUP(E102, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="8">
+      <c r="A103" s="9">
         <v>98.0</v>
       </c>
-      <c r="D103" s="11"/>
-      <c r="E103" s="10">
-        <f>IFERROR(VLOOKUP(D103, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B103" s="12"/>
+      <c r="C103" s="10"/>
+      <c r="D103" s="12"/>
+      <c r="E103" s="12"/>
+      <c r="F103" s="11">
+        <f>IFERROR(VLOOKUP(E103, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="8">
+      <c r="A104" s="9">
         <v>99.0</v>
       </c>
-      <c r="D104" s="11"/>
-      <c r="E104" s="10">
-        <f>IFERROR(VLOOKUP(D104, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B104" s="12"/>
+      <c r="C104" s="10"/>
+      <c r="D104" s="12"/>
+      <c r="E104" s="12"/>
+      <c r="F104" s="11">
+        <f>IFERROR(VLOOKUP(E104, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="8">
+      <c r="A105" s="9">
         <v>100.0</v>
       </c>
-      <c r="D105" s="11"/>
-      <c r="E105" s="10">
-        <f>IFERROR(VLOOKUP(D105, config!$A$2:$B$3, 2, FALSE), 0)</f>
+      <c r="B105" s="12"/>
+      <c r="C105" s="10"/>
+      <c r="D105" s="12"/>
+      <c r="E105" s="12"/>
+      <c r="F105" s="11">
+        <f>IFERROR(VLOOKUP(E105, config!$A$2:$B$3, 2, FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="8"/>
+      <c r="A106" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A4:F4"/>
   </mergeCells>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Clique ou digite um valor da lista de itens" sqref="D6:D105">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Clique ou digite um valor da lista de itens" sqref="E6:E105">
       <formula1>"Normal,Insenta"</formula1>
+    </dataValidation>
+    <dataValidation type="date" allowBlank="1" showDropDown="1" sqref="C6:C105">
+      <formula1>2.0</formula1>
+      <formula2>HOJE()</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D6:D105">
+      <formula1>"Mas,Fem"</formula1>
     </dataValidation>
   </dataValidations>
   <drawing r:id="rId1"/>
@@ -1494,26 +1821,26 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="8">
+      <c r="A2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="13">
         <v>160.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="8">
+      <c r="A3" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="13">
         <v>80.0</v>
       </c>
     </row>

</xml_diff>